<commit_message>
Adding automation code to git
</commit_message>
<xml_diff>
--- a/TestInputs/DTFO/InputSheet.xlsx
+++ b/TestInputs/DTFO/InputSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="126">
   <si>
     <t>TCID</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>quantityValidation</t>
+  </si>
+  <si>
+    <t>Wait for Quantity</t>
+  </si>
+  <si>
+    <t>Enter Invalid Quantity</t>
+  </si>
+  <si>
+    <t>/html/body/main/div[4]/section/div/div[2]/div[1]/div/ul/table/tbody/tr/td/li[1]/div[5]/form/input[4]</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:F23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,19 +2851,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2878,7 +2887,282 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>